<commit_message>
Solved logistic_reg problem, started lasso. Started gradient descent alg
</commit_message>
<xml_diff>
--- a/Feature_Selection.xlsx
+++ b/Feature_Selection.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="William" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="114">
   <si>
     <t xml:space="preserve">DER/PI</t>
   </si>
@@ -342,6 +342,15 @@
   </si>
   <si>
     <t xml:space="preserve">Intercept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log(+3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log(+1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log(+2)</t>
   </si>
   <si>
     <t xml:space="preserve">jet_num 0</t>
@@ -1435,7 +1444,7 @@
   <dimension ref="A1:Y58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1495,7 +1504,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="0" t="n">
-        <f aca="false"> E2+1</f>
+        <f aca="false">E2+1</f>
         <v>1</v>
       </c>
       <c r="G3" s="0" t="n">
@@ -1564,6 +1573,9 @@
         <f aca="false">E4+1</f>
         <v>3</v>
       </c>
+      <c r="F5" s="0" t="s">
+        <v>107</v>
+      </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -1594,6 +1606,9 @@
         <f aca="false">E5+1</f>
         <v>4</v>
       </c>
+      <c r="F6" s="0" t="s">
+        <v>108</v>
+      </c>
       <c r="K6" s="3" t="s">
         <v>11</v>
       </c>
@@ -1693,6 +1708,9 @@
         <f aca="false">E10+1</f>
         <v>9</v>
       </c>
+      <c r="F11" s="0" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -1785,6 +1803,9 @@
         <f aca="false">E15+1</f>
         <v>14</v>
       </c>
+      <c r="F16" s="0" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
@@ -1842,6 +1863,9 @@
         <f aca="false">E18+1</f>
         <v>17</v>
       </c>
+      <c r="F19" s="0" t="s">
+        <v>108</v>
+      </c>
       <c r="K19" s="5" t="s">
         <v>33</v>
       </c>
@@ -1902,6 +1926,9 @@
         <f aca="false">E21+1</f>
         <v>20</v>
       </c>
+      <c r="F22" s="0" t="s">
+        <v>109</v>
+      </c>
       <c r="K22" s="5" t="s">
         <v>39</v>
       </c>
@@ -1971,6 +1998,9 @@
         <f aca="false">E24+1</f>
         <v>23</v>
       </c>
+      <c r="F26" s="0" t="s">
+        <v>109</v>
+      </c>
       <c r="G26" s="3" t="n">
         <v>39</v>
       </c>
@@ -2109,13 +2139,16 @@
         <f aca="false">E31+1</f>
         <v>29</v>
       </c>
+      <c r="F32" s="0" t="s">
+        <v>108</v>
+      </c>
       <c r="K32" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E33" s="0" t="n">
         <f aca="false">E32+1</f>
@@ -2125,7 +2158,7 @@
     </row>
     <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E34" s="0" t="n">
         <f aca="false">E33+1</f>
@@ -2135,7 +2168,7 @@
     </row>
     <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E35" s="0" t="n">
         <f aca="false">E34+1</f>
@@ -2145,7 +2178,7 @@
     </row>
     <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E36" s="0" t="n">
         <f aca="false">E35+1</f>

</xml_diff>

<commit_message>
Final Result Generation Preparation
</commit_message>
<xml_diff>
--- a/Feature_Selection.xlsx
+++ b/Feature_Selection.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Marie/Documents/Github/ML_CS433_projet1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5008DE2F-2B60-D047-A528-18DDAEB5B537}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12458180-E88E-2742-9658-1B960434FD4A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="28620" windowHeight="16240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="740" windowWidth="25600" windowHeight="16240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="William" sheetId="2" r:id="rId2"/>
     <sheet name="Matrix" sheetId="3" r:id="rId3"/>
     <sheet name="Lasso" sheetId="4" r:id="rId4"/>
+    <sheet name="Big Table" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179021" iterateDelta="1E-4"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="170">
   <si>
     <t>DER/PI</t>
   </si>
@@ -474,9 +475,6 @@
     <t>I need to rerun ~</t>
   </si>
   <si>
-    <t>I need to rerun, ~ 0.23</t>
-  </si>
-  <si>
     <t>Least Squares</t>
   </si>
   <si>
@@ -502,13 +500,52 @@
   </si>
   <si>
     <t>I need to rerun ~0.21</t>
+  </si>
+  <si>
+    <t>Least squares (GD)</t>
+  </si>
+  <si>
+    <t>Least squares (SGD)</t>
+  </si>
+  <si>
+    <t>Ridge regression</t>
+  </si>
+  <si>
+    <t>Logistic regression (GD)</t>
+  </si>
+  <si>
+    <t>Regularized logistic regression (GD)</t>
+  </si>
+  <si>
+    <t>Least squares         (normal equations)</t>
+  </si>
+  <si>
+    <t>Training data</t>
+  </si>
+  <si>
+    <t>Imputation method</t>
+  </si>
+  <si>
+    <t>Neutral</t>
+  </si>
+  <si>
+    <t>Logarithmic</t>
+  </si>
+  <si>
+    <t>Interaction</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Test loss mean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -582,6 +619,19 @@
       <color rgb="FF47494D"/>
       <name val="Inherit"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -621,7 +671,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -629,11 +679,111 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -653,6 +803,41 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1923,11 +2108,11 @@
         <v>111</v>
       </c>
       <c r="D3">
-        <f>D2+1</f>
+        <f t="shared" ref="D3:D23" si="0">D2+1</f>
         <v>1</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E19" si="0">E2+1</f>
+        <f t="shared" ref="E3:E19" si="1">E2+1</f>
         <v>1</v>
       </c>
     </row>
@@ -1936,11 +2121,11 @@
         <v>112</v>
       </c>
       <c r="D4">
-        <f>D3+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -1949,11 +2134,11 @@
         <v>113</v>
       </c>
       <c r="D5">
-        <f>D4+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -1966,11 +2151,11 @@
       </c>
       <c r="C6" s="7"/>
       <c r="D6">
-        <f>D5+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="G6" s="7"/>
@@ -1980,15 +2165,15 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B7:B35" si="1">B6+1</f>
+        <f t="shared" ref="B7:B35" si="2">B6+1</f>
         <v>1</v>
       </c>
       <c r="D7">
-        <f>D6+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="G7">
@@ -2017,15 +2202,15 @@
         <v>9</v>
       </c>
       <c r="B8">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <f>D7+1</f>
-        <v>6</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L8" s="2"/>
@@ -2048,18 +2233,18 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C9" t="s">
         <v>107</v>
       </c>
       <c r="D9">
-        <f>D8+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="L9" s="2"/>
@@ -2082,15 +2267,15 @@
         <v>12</v>
       </c>
       <c r="B10">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <f>D9+1</f>
-        <v>8</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="K10" s="3" t="s">
@@ -2103,18 +2288,18 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="C11" t="s">
         <v>117</v>
       </c>
       <c r="D11">
-        <f>D10+1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -2123,15 +2308,15 @@
         <v>16</v>
       </c>
       <c r="B12">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E12">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="D12">
-        <f>D11+1</f>
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="K12" s="4" t="s">
@@ -2143,15 +2328,15 @@
         <v>18</v>
       </c>
       <c r="B13">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E13">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="D13">
-        <f>D12+1</f>
-        <v>11</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="K13" s="4" t="s">
@@ -2163,18 +2348,18 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="C14" t="s">
         <v>108</v>
       </c>
       <c r="D14">
-        <f>D13+1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
@@ -2183,18 +2368,18 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="C15" t="s">
         <v>117</v>
       </c>
       <c r="D15">
-        <f>D14+1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
@@ -2203,15 +2388,15 @@
         <v>22</v>
       </c>
       <c r="B16">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E16">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="D16">
-        <f>D15+1</f>
-        <v>14</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="K16" t="s">
@@ -2223,15 +2408,15 @@
         <v>23</v>
       </c>
       <c r="B17">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E17">
         <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="D17">
-        <f>D16+1</f>
-        <v>15</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -2240,15 +2425,15 @@
         <v>25</v>
       </c>
       <c r="B18">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E18">
         <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="D18">
-        <f>D17+1</f>
-        <v>16</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="H18" t="s">
@@ -2263,18 +2448,18 @@
         <v>26</v>
       </c>
       <c r="B19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="C19" t="s">
         <v>108</v>
       </c>
       <c r="D19">
-        <f>D18+1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
     </row>
@@ -2283,11 +2468,11 @@
         <v>28</v>
       </c>
       <c r="B20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="D20">
-        <f>D19+1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -2296,11 +2481,11 @@
         <v>30</v>
       </c>
       <c r="B21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="D21">
-        <f>D20+1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="K21" s="5" t="s">
@@ -2312,14 +2497,14 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="C22" t="s">
         <v>108</v>
       </c>
       <c r="D22">
-        <f>D21+1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="E22">
@@ -2338,11 +2523,11 @@
         <v>34</v>
       </c>
       <c r="B23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="D23">
-        <f>D22+1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="K23" s="5" t="s">
@@ -2354,7 +2539,7 @@
         <v>36</v>
       </c>
       <c r="B24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="D24">
@@ -2370,7 +2555,7 @@
         <v>38</v>
       </c>
       <c r="B25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="C25" t="s">
@@ -2396,7 +2581,7 @@
         <v>40</v>
       </c>
       <c r="B26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="D26">
@@ -2412,7 +2597,7 @@
         <v>41</v>
       </c>
       <c r="B27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="D27">
@@ -2428,7 +2613,7 @@
         <v>43</v>
       </c>
       <c r="B28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="K28" s="5" t="s">
@@ -2440,7 +2625,7 @@
         <v>44</v>
       </c>
       <c r="B29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="C29" t="s">
@@ -2460,7 +2645,7 @@
         <v>46</v>
       </c>
       <c r="B30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="D30">
@@ -2479,7 +2664,7 @@
         <v>48</v>
       </c>
       <c r="B31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="D31">
@@ -2498,7 +2683,7 @@
         <v>50</v>
       </c>
       <c r="B32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="C32" t="s">
@@ -2526,7 +2711,7 @@
         <v>52</v>
       </c>
       <c r="B33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="D33">
@@ -2541,7 +2726,7 @@
         <v>54</v>
       </c>
       <c r="B34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="D34">
@@ -2556,7 +2741,7 @@
         <v>56</v>
       </c>
       <c r="B35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="C35" t="s">
@@ -2670,7 +2855,7 @@
         <v>74</v>
       </c>
       <c r="E47" t="e">
-        <f t="shared" ref="E47" si="2">E46+1</f>
+        <f t="shared" ref="E47" si="3">E46+1</f>
         <v>#REF!</v>
       </c>
       <c r="F47" s="1"/>
@@ -2824,8 +3009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE807B20-13FC-1340-B171-6F7DDEED2EC0}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2962,7 +3147,7 @@
         <v>0.75405</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>10</v>
@@ -3004,7 +3189,7 @@
         <v>0.73912</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>12</v>
@@ -3043,7 +3228,7 @@
         <v>0.75561</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>14</v>
@@ -3079,7 +3264,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>16</v>
@@ -3112,7 +3297,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>18</v>
@@ -3145,7 +3330,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>19</v>
@@ -3181,7 +3366,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>20</v>
@@ -3220,7 +3405,7 @@
         <v>1</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>22</v>
@@ -3232,7 +3417,7 @@
     </row>
     <row r="13" spans="1:14" ht="19">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B13" t="s">
         <v>143</v>
@@ -3256,7 +3441,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L13" s="18" t="s">
         <v>23</v>
@@ -3286,13 +3471,13 @@
         <v>136</v>
       </c>
       <c r="G14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>25</v>
@@ -3323,7 +3508,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="12:14" ht="19">
+    <row r="17" spans="1:14" ht="19">
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
       <c r="L17" s="11" t="s">
         <v>30</v>
       </c>
@@ -3332,7 +3520,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="12:14" ht="19">
+    <row r="18" spans="1:14" ht="19">
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
       <c r="L18" s="1" t="s">
         <v>32</v>
       </c>
@@ -3344,7 +3535,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="12:14" ht="19">
+    <row r="19" spans="1:14" ht="19">
       <c r="L19" s="10" t="s">
         <v>34</v>
       </c>
@@ -3353,7 +3544,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="12:14" ht="19">
+    <row r="20" spans="1:14" ht="19">
       <c r="L20" s="11" t="s">
         <v>36</v>
       </c>
@@ -3362,7 +3553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="12:14" ht="19">
+    <row r="21" spans="1:14" ht="19">
       <c r="L21" s="1" t="s">
         <v>38</v>
       </c>
@@ -3374,7 +3565,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="12:14" ht="19">
+    <row r="22" spans="1:14" ht="19">
       <c r="L22" s="11" t="s">
         <v>40</v>
       </c>
@@ -3383,7 +3574,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="12:14" ht="19">
+    <row r="23" spans="1:14" ht="19">
       <c r="L23" s="11" t="s">
         <v>41</v>
       </c>
@@ -3392,7 +3583,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="12:14" ht="19">
+    <row r="24" spans="1:14" ht="19">
       <c r="L24" s="1" t="s">
         <v>43</v>
       </c>
@@ -3401,7 +3592,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="12:14" ht="19">
+    <row r="25" spans="1:14" ht="19">
       <c r="L25" s="1" t="s">
         <v>44</v>
       </c>
@@ -3413,7 +3604,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="12:14" ht="19">
+    <row r="26" spans="1:14" ht="19">
       <c r="L26" s="12" t="s">
         <v>46</v>
       </c>
@@ -3422,7 +3613,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="12:14" ht="19">
+    <row r="27" spans="1:14" ht="19">
       <c r="L27" s="10" t="s">
         <v>48</v>
       </c>
@@ -3431,7 +3622,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="12:14" ht="19">
+    <row r="28" spans="1:14" ht="19">
       <c r="L28" s="1" t="s">
         <v>50</v>
       </c>
@@ -3443,7 +3634,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="12:14" ht="19">
+    <row r="29" spans="1:14" ht="19">
       <c r="L29" s="10" t="s">
         <v>52</v>
       </c>
@@ -3452,7 +3643,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="12:14" ht="19">
+    <row r="30" spans="1:14" ht="19">
       <c r="L30" s="10" t="s">
         <v>54</v>
       </c>
@@ -3461,7 +3652,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="12:14" ht="19">
+    <row r="31" spans="1:14" ht="19">
       <c r="L31" s="1" t="s">
         <v>56</v>
       </c>
@@ -3482,8 +3673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF10F3A-46DA-7B40-800D-0CCA7C91A5A0}">
   <dimension ref="A2:J43"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3590,7 +3781,7 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <f>B11+1</f>
+        <f t="shared" ref="B12:B32" si="0">B11+1</f>
         <v>1</v>
       </c>
       <c r="C12" s="16">
@@ -3602,7 +3793,7 @@
         <v>9</v>
       </c>
       <c r="B13">
-        <f>B12+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C13" s="16">
@@ -3614,7 +3805,7 @@
         <v>10</v>
       </c>
       <c r="B14">
-        <f>B13+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C14" s="16">
@@ -3626,7 +3817,7 @@
         <v>12</v>
       </c>
       <c r="B15">
-        <f>B14+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C15" s="16">
@@ -3638,7 +3829,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <f>B15+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C16" s="16">
@@ -3650,7 +3841,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <f>B16+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C17" s="16">
@@ -3662,7 +3853,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <f>B17+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C18" s="16">
@@ -3674,7 +3865,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <f>B18+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C19" s="16">
@@ -3686,7 +3877,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <f>B19+1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C20" s="16">
@@ -3698,7 +3889,7 @@
         <v>22</v>
       </c>
       <c r="B21">
-        <f>B20+1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C21" s="16">
@@ -3710,7 +3901,7 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <f>B21+1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C22" s="16">
@@ -3722,7 +3913,7 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <f>B22+1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C23" s="16">
@@ -3734,7 +3925,7 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <f>B23+1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C24" s="16">
@@ -3746,7 +3937,7 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <f>B24+1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C25" s="16">
@@ -3758,7 +3949,7 @@
         <v>30</v>
       </c>
       <c r="B26">
-        <f>B25+1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C26" s="16">
@@ -3770,7 +3961,7 @@
         <v>32</v>
       </c>
       <c r="B27">
-        <f>B26+1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C27" s="16">
@@ -3782,7 +3973,7 @@
         <v>34</v>
       </c>
       <c r="B28">
-        <f>B27+1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="C28" s="16">
@@ -3794,7 +3985,7 @@
         <v>36</v>
       </c>
       <c r="B29">
-        <f>B28+1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="C29" s="16">
@@ -3806,7 +3997,7 @@
         <v>38</v>
       </c>
       <c r="B30">
-        <f>B29+1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="C30" s="16">
@@ -3818,7 +4009,7 @@
         <v>40</v>
       </c>
       <c r="B31">
-        <f>B30+1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C31" s="16">
@@ -3830,7 +4021,7 @@
         <v>41</v>
       </c>
       <c r="B32">
-        <f>B31+1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C32" s="16">
@@ -3853,7 +4044,7 @@
         <v>46</v>
       </c>
       <c r="B34">
-        <f>B33+1</f>
+        <f t="shared" ref="B34:B39" si="1">B33+1</f>
         <v>24</v>
       </c>
       <c r="C34" s="16">
@@ -3865,7 +4056,7 @@
         <v>48</v>
       </c>
       <c r="B35">
-        <f>B34+1</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="C35" s="16">
@@ -3877,7 +4068,7 @@
         <v>50</v>
       </c>
       <c r="B36">
-        <f>B35+1</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="C36" s="16">
@@ -3889,7 +4080,7 @@
         <v>52</v>
       </c>
       <c r="B37">
-        <f>B36+1</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="C37" s="16">
@@ -3901,7 +4092,7 @@
         <v>54</v>
       </c>
       <c r="B38">
-        <f>B37+1</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C38" s="16">
@@ -3913,7 +4104,7 @@
         <v>56</v>
       </c>
       <c r="B39">
-        <f>B38+1</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="C39" s="16">
@@ -3967,4 +4158,157 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA45F76-1072-124A-8C3B-8E843CBF4B12}">
+  <dimension ref="B2:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10">
+      <c r="B2" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" s="27"/>
+      <c r="E2" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="27"/>
+      <c r="G2" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="H2" s="38"/>
+      <c r="I2" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="J2" s="25"/>
+    </row>
+    <row r="3" spans="2:10" ht="17" thickBot="1">
+      <c r="B3" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="17">
+      <c r="B4" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="37"/>
+    </row>
+    <row r="5" spans="2:10" ht="17">
+      <c r="B5" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="37"/>
+    </row>
+    <row r="6" spans="2:10" ht="34">
+      <c r="B6" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="37"/>
+    </row>
+    <row r="7" spans="2:10" ht="17">
+      <c r="B7" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="37"/>
+    </row>
+    <row r="8" spans="2:10" ht="17">
+      <c r="B8" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="37"/>
+    </row>
+    <row r="9" spans="2:10" ht="35" thickBot="1">
+      <c r="B9" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+    </row>
+    <row r="10" spans="2:10" ht="17">
+      <c r="B10" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="37"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>